<commit_message>
new file:   Eurazeo/Companies.xlsx new file:   Eurazeo/Eurazeo Portfolio.py new file:   Eurazeo/test.py modified:   Insight Partners/Companies.xlsx modified:   Insight Partners/Insight Partners Portfolio.py
</commit_message>
<xml_diff>
--- a/Insight Partners/Companies.xlsx
+++ b/Insight Partners/Companies.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://2xmarketing-my.sharepoint.com/personal/rajveer_singh_2x_marketing/Documents/Workspcace VS Code/GitHub Repos/Insight Partners Web Scraping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://2xmarketing-my.sharepoint.com/personal/rajveer_singh_2x_marketing/Documents/Workspcace VS Code/GitHub Repos/WebScraper/Insight Partners/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_106161E760AB0B8B572273FB55083121787681CD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F80A83B-B5D3-4621-8F1F-36234E07557E}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_106161E760AB0B8B572273FB55083121787681CD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FF4D39B-B748-47FC-949D-62D39A847CB6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13281,8 +13281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M509"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13291,6 +13291,7 @@
     <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="118.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="38.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="101.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="86.109375" bestFit="1" customWidth="1"/>

</xml_diff>